<commit_message>
Generate responses to test questions
</commit_message>
<xml_diff>
--- a/data/RAG+C_Q&A.xlsx
+++ b/data/RAG+C_Q&A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/GitHub/dl-tutorial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6984C8B-8C6D-9D4E-9277-CD7F94E73DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C810C85-A154-5E4A-B2A8-05AD497CCE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A99B8B7A-6E4F-D340-AB46-64BDB3A6AE93}"/>
   </bookViews>
@@ -38,18 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="136">
   <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>Response with Context</t>
-  </si>
-  <si>
-    <t>Response without Context</t>
-  </si>
-  <si>
     <t>True or False? Contractors who provide products or services to the Federal Government are to be considered members of the Government’s “Federal Acquisition Team.”</t>
   </si>
   <si>
@@ -68,9 +56,6 @@
     <t>FAR 1.102-2 provides that the principal customers are “the users and line managers acting on behalf of the American tax payer.”</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>What is the FAR?</t>
   </si>
   <si>
@@ -317,9 +302,6 @@
     <t xml:space="preserve">https://publiccontractinginstitute.com/far-knowledge-test/ </t>
   </si>
   <si>
-    <t>Question (edited)</t>
-  </si>
-  <si>
     <t>Is it true that contractors who provide products or services to the Federal Government are to be considered members of the Government’s “Federal Acquisition Team”?</t>
   </si>
   <si>
@@ -353,9 +335,6 @@
     <t xml:space="preserve">(TRUE or FALSE) As a general rule, a Government employee may not solicit any gift or gratuity from anyone seeking to obtain Government business, but may accept monetary gifts and entertainment as long as they are not solicited. </t>
   </si>
   <si>
-    <t>Can Government employees accept monetary gfts and entertainment from someone seeking to obtain Government business as long as they are not solicited?</t>
-  </si>
-  <si>
     <t>What is a contingent fee?</t>
   </si>
   <si>
@@ -444,6 +423,27 @@
   </si>
   <si>
     <t>What are the responsibilities of the Contracting Officer?</t>
+  </si>
+  <si>
+    <t>response_context</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>question_edited</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>response_no_context</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Can Government employees accept monetary gifts and entertainment from someone seeking to obtain Government business as long as they are not solicited?</t>
   </si>
 </sst>
 </file>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535A2AB0-AF37-8049-9E87-8610FCDC68CD}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="117" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,722 +854,722 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>129</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1">
         <v>30</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculate avg similarity scores
</commit_message>
<xml_diff>
--- a/data/RAG+C_Q&A.xlsx
+++ b/data/RAG+C_Q&A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/GitHub/dl-tutorial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C810C85-A154-5E4A-B2A8-05AD497CCE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82D8F07-60F7-814D-9EFB-BA3202F0D342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A99B8B7A-6E4F-D340-AB46-64BDB3A6AE93}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="139">
   <si>
     <t>True or False? Contractors who provide products or services to the Federal Government are to be considered members of the Government’s “Federal Acquisition Team.”</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>Can Government employees accept monetary gifts and entertainment from someone seeking to obtain Government business as long as they are not solicited?</t>
+  </si>
+  <si>
+    <t>answer_edited</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Thirty days.</t>
   </si>
 </sst>
 </file>
@@ -836,23 +845,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535A2AB0-AF37-8049-9E87-8610FCDC68CD}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="117" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="48" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="4" width="48" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>132</v>
       </c>
@@ -862,17 +871,20 @@
       <c r="C1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -882,11 +894,14 @@
       <c r="C2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -896,11 +911,14 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -910,11 +928,14 @@
       <c r="C4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -924,11 +945,14 @@
       <c r="C5" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -938,11 +962,14 @@
       <c r="C6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -952,11 +979,14 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -966,11 +996,14 @@
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -980,11 +1013,14 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>96</v>
       </c>
@@ -994,11 +1030,14 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>98</v>
       </c>
@@ -1008,11 +1047,14 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1022,11 +1064,14 @@
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1036,11 +1081,14 @@
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1050,11 +1098,14 @@
       <c r="C14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>104</v>
       </c>
@@ -1064,11 +1115,14 @@
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>103</v>
       </c>
@@ -1078,11 +1132,14 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1092,11 +1149,14 @@
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1106,11 +1166,14 @@
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1120,11 +1183,14 @@
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1134,11 +1200,14 @@
       <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1148,11 +1217,14 @@
       <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1162,11 +1234,14 @@
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -1176,11 +1251,14 @@
       <c r="C23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -1190,11 +1268,14 @@
       <c r="C24" s="1">
         <v>3</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -1204,11 +1285,14 @@
       <c r="C25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -1218,11 +1302,14 @@
       <c r="C26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1232,11 +1319,14 @@
       <c r="C27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
@@ -1246,11 +1336,14 @@
       <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
@@ -1260,11 +1353,14 @@
       <c r="C29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="D29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
@@ -1274,11 +1370,14 @@
       <c r="C30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -1288,11 +1387,14 @@
       <c r="C31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
@@ -1302,11 +1404,14 @@
       <c r="C32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
@@ -1316,11 +1421,14 @@
       <c r="C33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
@@ -1330,11 +1438,14 @@
       <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>59</v>
       </c>
@@ -1344,11 +1455,14 @@
       <c r="C35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
@@ -1358,11 +1472,14 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
@@ -1372,11 +1489,14 @@
       <c r="C37" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>65</v>
       </c>
@@ -1386,11 +1506,14 @@
       <c r="C38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -1400,11 +1523,14 @@
       <c r="C39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>69</v>
       </c>
@@ -1414,11 +1540,14 @@
       <c r="C40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>71</v>
       </c>
@@ -1428,11 +1557,14 @@
       <c r="C41" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>73</v>
       </c>
@@ -1442,11 +1574,14 @@
       <c r="C42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="D42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>119</v>
       </c>
@@ -1456,11 +1591,14 @@
       <c r="C43" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>76</v>
       </c>
@@ -1470,11 +1608,14 @@
       <c r="C44" s="1">
         <v>30</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>76</v>
       </c>
@@ -1484,11 +1625,14 @@
       <c r="C45" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>77</v>
       </c>
@@ -1498,11 +1642,14 @@
       <c r="C46" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>79</v>
       </c>
@@ -1512,11 +1659,14 @@
       <c r="C47" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>81</v>
       </c>
@@ -1526,11 +1676,14 @@
       <c r="C48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D48" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>83</v>
       </c>
@@ -1540,11 +1693,14 @@
       <c r="C49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="D49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>85</v>
       </c>
@@ -1554,11 +1710,14 @@
       <c r="C50" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>43</v>
       </c>
@@ -1568,15 +1727,14 @@
       <c r="C51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="D51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1" xr:uid="{BDC3A757-724A-AA40-B907-D6FF7D5D6DF2}"/>
-    <hyperlink ref="F26" r:id="rId2" xr:uid="{9EE13346-6B38-314E-9EB4-981AC62E4DE3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>